<commit_message>
Update lab number and date in main.tex
</commit_message>
<xml_diff>
--- a/Lab 7/07_Flow_Data_Collection_Tables.xlsx
+++ b/Lab 7/07_Flow_Data_Collection_Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\LaTeX\MEC-E-301\Lab 7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59955C3-4C34-4491-8358-9110B8DBB664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207BF9D2-AE4C-4510-840F-20B161A0C4E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -606,12 +606,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
-    <numFmt numFmtId="169" formatCode="0.0000000"/>
-    <numFmt numFmtId="170" formatCode="0.000"/>
-    <numFmt numFmtId="173" formatCode="0.0"/>
-    <numFmt numFmtId="174" formatCode="0.0000"/>
-    <numFmt numFmtId="176" formatCode="0.00000"/>
-    <numFmt numFmtId="179" formatCode="0.0E+00"/>
+    <numFmt numFmtId="164" formatCode="0.0000000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="168" formatCode="0.00000"/>
+    <numFmt numFmtId="169" formatCode="0.0E+00"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -752,7 +752,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -826,6 +826,25 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -847,31 +866,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="173" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="173" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1310,8 +1304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B5A20CD-CFFA-604A-B1A6-58C924DA13F1}">
   <dimension ref="A1:Y99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1530,7 +1524,7 @@
       <c r="J17" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="K17" s="38" cm="1">
+      <c r="K17" s="30" cm="1">
         <f t="array" ref="K17:L21">LINEST(B56:B65,A56:A65, TRUE, TRUE)</f>
         <v>0.26600136085280102</v>
       </c>
@@ -1626,22 +1620,22 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="29" t="s">
+      <c r="A24" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="29"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="J24" s="45">
+      <c r="B24" s="42"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="J24" s="36">
         <v>0.60115999999999903</v>
       </c>
-      <c r="K24" s="39">
+      <c r="K24" s="31">
         <v>5.147185403641517E-4</v>
       </c>
-      <c r="L24" s="39">
+      <c r="L24" s="31">
         <v>1662.6969000000001</v>
       </c>
-      <c r="M24" s="41">
+      <c r="M24" s="33">
         <v>1.6892795452369394E-2</v>
       </c>
     </row>
@@ -1658,21 +1652,21 @@
       <c r="D25" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="J25" s="46">
+      <c r="J25" s="37">
         <v>0.60143999999999997</v>
       </c>
-      <c r="K25" s="39">
+      <c r="K25" s="31">
         <v>5.147185403641517E-4</v>
       </c>
-      <c r="L25" s="39">
+      <c r="L25" s="31">
         <v>1310.5963800000002</v>
       </c>
-      <c r="M25" s="41">
+      <c r="M25" s="33">
         <v>1.5004851252418554E-2</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="30" t="s">
+      <c r="A26" s="43" t="s">
         <v>22</v>
       </c>
       <c r="B26" s="16">
@@ -1684,21 +1678,21 @@
       <c r="D26" s="16">
         <v>10.5</v>
       </c>
-      <c r="J26" s="46">
+      <c r="J26" s="37">
         <v>0.60161600000000004</v>
       </c>
-      <c r="K26" s="39">
+      <c r="K26" s="31">
         <v>5.147185403641517E-4</v>
       </c>
-      <c r="L26" s="39">
+      <c r="L26" s="31">
         <v>1075.8627000000001</v>
       </c>
-      <c r="M26" s="41">
+      <c r="M26" s="33">
         <v>1.35988664060776E-2</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="31"/>
+      <c r="A27" s="44"/>
       <c r="B27" s="13">
         <v>120</v>
       </c>
@@ -1708,21 +1702,21 @@
       <c r="D27" s="13">
         <v>13.5</v>
       </c>
-      <c r="J27" s="46">
+      <c r="J27" s="37">
         <v>0.60186200000000001</v>
       </c>
-      <c r="K27" s="39">
+      <c r="K27" s="31">
         <v>5.147185403641517E-4</v>
       </c>
-      <c r="L27" s="47">
+      <c r="L27" s="38">
         <v>821.56788000000006</v>
       </c>
-      <c r="M27" s="41">
+      <c r="M27" s="33">
         <v>1.1888403966416864E-2</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="31"/>
+      <c r="A28" s="44"/>
       <c r="B28" s="13">
         <v>125</v>
       </c>
@@ -1732,21 +1726,21 @@
       <c r="D28" s="13">
         <v>17</v>
       </c>
-      <c r="J28" s="46">
+      <c r="J28" s="37">
         <v>0.60233599999999998</v>
       </c>
-      <c r="K28" s="39">
+      <c r="K28" s="31">
         <v>5.147185403641517E-4</v>
       </c>
-      <c r="L28" s="47">
+      <c r="L28" s="38">
         <v>616.17591000000004</v>
       </c>
-      <c r="M28" s="41">
+      <c r="M28" s="33">
         <v>1.0303768253553129E-2</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="31"/>
+      <c r="A29" s="44"/>
       <c r="B29" s="13">
         <v>135</v>
       </c>
@@ -1756,21 +1750,21 @@
       <c r="D29" s="13">
         <v>19</v>
       </c>
-      <c r="J29" s="46">
+      <c r="J29" s="37">
         <v>0.60289999999999999</v>
       </c>
-      <c r="K29" s="39">
+      <c r="K29" s="31">
         <v>5.147185403641517E-4</v>
       </c>
-      <c r="L29" s="47">
+      <c r="L29" s="38">
         <v>420.56451000000004</v>
       </c>
-      <c r="M29" s="46">
+      <c r="M29" s="37">
         <v>8.5205278163054867E-3</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="32"/>
+      <c r="A30" s="45"/>
       <c r="B30" s="14">
         <v>140</v>
       </c>
@@ -1780,16 +1774,16 @@
       <c r="D30" s="14">
         <v>19</v>
       </c>
-      <c r="J30" s="46">
+      <c r="J30" s="37">
         <v>0.60348000000000002</v>
       </c>
-      <c r="K30" s="39">
+      <c r="K30" s="31">
         <v>5.147185403641517E-4</v>
       </c>
-      <c r="L30" s="47">
+      <c r="L30" s="38">
         <v>312.97824000000003</v>
       </c>
-      <c r="M30" s="46">
+      <c r="M30" s="37">
         <v>7.3574082974058102E-3</v>
       </c>
     </row>
@@ -1806,21 +1800,21 @@
       <c r="D31" s="15">
         <v>18.5</v>
       </c>
-      <c r="J31" s="46">
+      <c r="J31" s="37">
         <v>0.60458000000000001</v>
       </c>
-      <c r="K31" s="39">
+      <c r="K31" s="31">
         <v>5.147185403641517E-4</v>
       </c>
-      <c r="L31" s="47">
+      <c r="L31" s="38">
         <v>200.50168500000001</v>
       </c>
-      <c r="M31" s="46">
+      <c r="M31" s="37">
         <v>5.8995338009355854E-3</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="30" t="s">
+      <c r="A32" s="43" t="s">
         <v>24</v>
       </c>
       <c r="B32" s="16">
@@ -1832,21 +1826,21 @@
       <c r="D32" s="16">
         <v>19.5</v>
       </c>
-      <c r="J32" s="46">
+      <c r="J32" s="37">
         <v>0.60646999999999995</v>
       </c>
-      <c r="K32" s="39">
+      <c r="K32" s="31">
         <v>5.147185403641517E-4</v>
       </c>
-      <c r="L32" s="47">
+      <c r="L32" s="38">
         <v>107.58627000000001</v>
       </c>
-      <c r="M32" s="46">
+      <c r="M32" s="37">
         <v>4.3350354389421128E-3</v>
       </c>
     </row>
     <row r="33" spans="1:25" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A33" s="31"/>
+      <c r="A33" s="44"/>
       <c r="B33" s="13">
         <v>155</v>
       </c>
@@ -1856,21 +1850,21 @@
       <c r="D33" s="13">
         <v>19.5</v>
       </c>
-      <c r="J33" s="46">
+      <c r="J33" s="37">
         <v>0.60950000000000004</v>
       </c>
-      <c r="K33" s="39">
+      <c r="K33" s="31">
         <v>5.147185403641517E-4</v>
       </c>
-      <c r="L33" s="40">
+      <c r="L33" s="32">
         <v>48.902850000000001</v>
       </c>
-      <c r="M33" s="46">
+      <c r="M33" s="37">
         <v>2.9372823731488086E-3</v>
       </c>
     </row>
     <row r="34" spans="1:25" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A34" s="31"/>
+      <c r="A34" s="44"/>
       <c r="B34" s="13">
         <v>165</v>
       </c>
@@ -1882,7 +1876,7 @@
       </c>
     </row>
     <row r="35" spans="1:25" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A35" s="31"/>
+      <c r="A35" s="44"/>
       <c r="B35" s="13">
         <v>170</v>
       </c>
@@ -1897,7 +1891,7 @@
       </c>
     </row>
     <row r="36" spans="1:25" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="32"/>
+      <c r="A36" s="45"/>
       <c r="B36" s="13">
         <v>180</v>
       </c>
@@ -1936,19 +1930,19 @@
       <c r="J37" t="s">
         <v>91</v>
       </c>
-      <c r="K37" s="41">
+      <c r="K37" s="33">
         <v>3.8302298336539642E-2</v>
       </c>
-      <c r="L37" s="41">
+      <c r="L37" s="33">
         <v>3.8302298336539642E-2</v>
       </c>
       <c r="N37" t="s">
         <v>41</v>
       </c>
-      <c r="O37" s="41">
+      <c r="O37" s="33">
         <v>3.8302298336539642E-2</v>
       </c>
-      <c r="P37" s="37">
+      <c r="P37" s="29">
         <v>1662.6969000000001</v>
       </c>
       <c r="Q37">
@@ -1957,7 +1951,7 @@
       <c r="R37">
         <v>7.2106619983356324E-4</v>
       </c>
-      <c r="S37" s="37">
+      <c r="S37" s="29">
         <v>0.95965779940048235</v>
       </c>
       <c r="T37">
@@ -1968,19 +1962,19 @@
       <c r="J38" t="s">
         <v>95</v>
       </c>
-      <c r="K38" s="37">
+      <c r="K38" s="29">
         <v>1662.6969000000001</v>
       </c>
-      <c r="L38" s="37">
+      <c r="L38" s="29">
         <v>3208.6200152400311</v>
       </c>
       <c r="N38" t="s">
         <v>96</v>
       </c>
-      <c r="O38" s="41">
+      <c r="O38" s="33">
         <v>3.8302298336539642E-2</v>
       </c>
-      <c r="P38" s="37">
+      <c r="P38" s="29">
         <v>3208.6200152400311</v>
       </c>
       <c r="Q38">
@@ -1989,7 +1983,7 @@
       <c r="R38">
         <v>5.147185403641517E-4</v>
       </c>
-      <c r="S38" s="37">
+      <c r="S38" s="29">
         <v>0.97438003710767163</v>
       </c>
       <c r="T38">
@@ -1997,12 +1991,12 @@
       </c>
     </row>
     <row r="39" spans="1:25" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="33" t="s">
+      <c r="A39" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="B39" s="33"/>
-      <c r="C39" s="33"/>
-      <c r="D39" s="33"/>
+      <c r="B39" s="46"/>
+      <c r="C39" s="46"/>
+      <c r="D39" s="46"/>
       <c r="J39" t="s">
         <v>97</v>
       </c>
@@ -2037,7 +2031,7 @@
       </c>
     </row>
     <row r="41" spans="1:25" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A41" s="30" t="s">
+      <c r="A41" s="43" t="s">
         <v>22</v>
       </c>
       <c r="B41" s="19">
@@ -2060,7 +2054,7 @@
       </c>
     </row>
     <row r="42" spans="1:25" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A42" s="31"/>
+      <c r="A42" s="44"/>
       <c r="B42" s="18">
         <v>-40</v>
       </c>
@@ -2081,7 +2075,7 @@
       </c>
     </row>
     <row r="43" spans="1:25" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A43" s="31"/>
+      <c r="A43" s="44"/>
       <c r="B43" s="18">
         <v>-30</v>
       </c>
@@ -2093,7 +2087,7 @@
       </c>
     </row>
     <row r="44" spans="1:25" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A44" s="31"/>
+      <c r="A44" s="44"/>
       <c r="B44" s="18">
         <v>-20</v>
       </c>
@@ -2105,7 +2099,7 @@
       </c>
     </row>
     <row r="45" spans="1:25" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A45" s="32"/>
+      <c r="A45" s="45"/>
       <c r="B45" s="20">
         <v>-10</v>
       </c>
@@ -2132,23 +2126,23 @@
       <c r="D46" s="15">
         <v>19.5</v>
       </c>
-      <c r="J46" s="27" t="s">
+      <c r="J46" s="40" t="s">
         <v>40</v>
       </c>
       <c r="K46" s="23"/>
       <c r="L46" s="23"/>
       <c r="M46" s="23"/>
-      <c r="N46" s="27" t="s">
+      <c r="N46" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="O46" s="27" t="s">
+      <c r="O46" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="P46" s="27"/>
+      <c r="P46" s="40"/>
       <c r="Q46" s="23"/>
     </row>
     <row r="47" spans="1:25" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A47" s="30" t="s">
+      <c r="A47" s="43" t="s">
         <v>24</v>
       </c>
       <c r="B47" s="19">
@@ -2160,17 +2154,17 @@
       <c r="D47" s="16">
         <v>19</v>
       </c>
-      <c r="J47" s="27"/>
+      <c r="J47" s="40"/>
       <c r="K47" s="23"/>
       <c r="L47" s="23"/>
       <c r="M47" s="23"/>
-      <c r="N47" s="27"/>
-      <c r="O47" s="28"/>
-      <c r="P47" s="28"/>
+      <c r="N47" s="40"/>
+      <c r="O47" s="41"/>
+      <c r="P47" s="41"/>
       <c r="Q47" s="23"/>
     </row>
     <row r="48" spans="1:25" ht="39" x14ac:dyDescent="0.25">
-      <c r="A48" s="31"/>
+      <c r="A48" s="44"/>
       <c r="B48" s="18">
         <v>20</v>
       </c>
@@ -2180,7 +2174,7 @@
       <c r="D48" s="13">
         <v>17</v>
       </c>
-      <c r="J48" s="28"/>
+      <c r="J48" s="41"/>
       <c r="K48" s="25" t="s">
         <v>48</v>
       </c>
@@ -2190,7 +2184,7 @@
       <c r="M48" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="N48" s="28"/>
+      <c r="N48" s="41"/>
       <c r="O48" s="24" t="s">
         <v>43</v>
       </c>
@@ -2200,16 +2194,16 @@
       <c r="Q48" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="R48" s="35" t="s">
+      <c r="R48" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="S48" s="35" t="s">
+      <c r="S48" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="T48" s="35" t="s">
+      <c r="T48" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="U48" s="35" t="s">
+      <c r="U48" s="23" t="s">
         <v>65</v>
       </c>
       <c r="V48" t="s">
@@ -2226,7 +2220,7 @@
       </c>
     </row>
     <row r="49" spans="1:25" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A49" s="31"/>
+      <c r="A49" s="44"/>
       <c r="B49" s="18">
         <v>30</v>
       </c>
@@ -2276,7 +2270,7 @@
         <f>_xlfn.XLOOKUP(L49, $A$4:$A$21, $B$4:$B$21, "not found", 1, 1)</f>
         <v>0.60289999999999999</v>
       </c>
-      <c r="V49" s="36">
+      <c r="V49" s="28">
         <f>IFERROR(FORECAST(K49,T49:U49,R49:S49), U49)</f>
         <v>0.60289999999999999</v>
       </c>
@@ -2294,7 +2288,7 @@
       </c>
     </row>
     <row r="50" spans="1:25" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A50" s="31"/>
+      <c r="A50" s="44"/>
       <c r="B50" s="18">
         <v>40</v>
       </c>
@@ -2306,7 +2300,7 @@
       </c>
     </row>
     <row r="51" spans="1:25" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A51" s="32"/>
+      <c r="A51" s="45"/>
       <c r="B51" s="20">
         <v>45</v>
       </c>
@@ -2345,10 +2339,10 @@
       </c>
     </row>
     <row r="54" spans="1:25" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="33" t="s">
+      <c r="A54" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="B54" s="33"/>
+      <c r="B54" s="46"/>
     </row>
     <row r="55" spans="1:25" ht="39.75" x14ac:dyDescent="0.2">
       <c r="A55" s="12" t="s">
@@ -2362,7 +2356,7 @@
       </c>
     </row>
     <row r="56" spans="1:25" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A56" s="43">
+      <c r="A56" s="34">
         <v>24.5</v>
       </c>
       <c r="B56" s="18">
@@ -2382,7 +2376,7 @@
       </c>
     </row>
     <row r="57" spans="1:25" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A57" s="43">
+      <c r="A57" s="34">
         <v>20</v>
       </c>
       <c r="B57" s="18">
@@ -2402,13 +2396,13 @@
         <f>0.5/100</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="N57" s="38">
+      <c r="N57" s="30">
         <f>SQRT(M57^2 + (1/2*K57)^2 + (1/2*L57)^2)</f>
         <v>1.3228756555322952E-2</v>
       </c>
     </row>
     <row r="58" spans="1:25" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A58" s="43">
+      <c r="A58" s="34">
         <v>17</v>
       </c>
       <c r="B58" s="18">
@@ -2427,13 +2421,13 @@
       <c r="M58" s="8">
         <v>0.02</v>
       </c>
-      <c r="N58" s="38">
+      <c r="N58" s="30">
         <f t="shared" ref="N58:N59" si="1">SQRT(M58^2 + (1/2*K58)^2 + (1/2*L58)^2)</f>
         <v>2.3452078799117149E-2</v>
       </c>
     </row>
     <row r="59" spans="1:25" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A59" s="43">
+      <c r="A59" s="34">
         <v>13</v>
       </c>
       <c r="B59" s="18">
@@ -2452,13 +2446,13 @@
       <c r="M59">
         <v>0.01</v>
       </c>
-      <c r="N59" s="38">
+      <c r="N59" s="30">
         <f t="shared" si="1"/>
         <v>1.5811388300841896E-2</v>
       </c>
     </row>
     <row r="60" spans="1:25" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A60" s="43">
+      <c r="A60" s="34">
         <v>10</v>
       </c>
       <c r="B60" s="18">
@@ -2466,7 +2460,7 @@
       </c>
     </row>
     <row r="61" spans="1:25" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A61" s="43">
+      <c r="A61" s="34">
         <v>9</v>
       </c>
       <c r="B61" s="18">
@@ -2477,13 +2471,13 @@
       </c>
     </row>
     <row r="62" spans="1:25" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A62" s="43">
+      <c r="A62" s="34">
         <v>6.5</v>
       </c>
       <c r="B62" s="18">
         <v>5.5</v>
       </c>
-      <c r="J62" s="48" cm="1">
+      <c r="J62" s="39" cm="1">
         <f t="array" ref="J62:K66">LINEST(D82:D91,P82:P91, TRUE, TRUE)</f>
         <v>16623.06994608137</v>
       </c>
@@ -2492,7 +2486,7 @@
       </c>
     </row>
     <row r="63" spans="1:25" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A63" s="43">
+      <c r="A63" s="34">
         <v>4.5</v>
       </c>
       <c r="B63" s="18">
@@ -2506,7 +2500,7 @@
       </c>
     </row>
     <row r="64" spans="1:25" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A64" s="43">
+      <c r="A64" s="34">
         <v>2</v>
       </c>
       <c r="B64" s="18">
@@ -2520,7 +2514,7 @@
       </c>
     </row>
     <row r="65" spans="1:17" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A65" s="44">
+      <c r="A65" s="35">
         <v>1</v>
       </c>
       <c r="B65" s="20">
@@ -2542,13 +2536,13 @@
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A68" s="29" t="s">
+      <c r="A68" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="B68" s="29"/>
-      <c r="C68" s="29"/>
-      <c r="D68" s="29"/>
-      <c r="E68" s="29"/>
+      <c r="B68" s="42"/>
+      <c r="C68" s="42"/>
+      <c r="D68" s="42"/>
+      <c r="E68" s="42"/>
     </row>
     <row r="69" spans="1:17" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A69" s="12" t="s">
@@ -2663,11 +2657,11 @@
       </c>
     </row>
     <row r="74" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="29" t="s">
+      <c r="A74" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="B74" s="29"/>
-      <c r="C74" s="29"/>
+      <c r="B74" s="42"/>
+      <c r="C74" s="42"/>
       <c r="I74" s="8" t="s">
         <v>66</v>
       </c>
@@ -2691,7 +2685,7 @@
       <c r="C75" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D75" s="42" t="s">
+      <c r="D75" s="9" t="s">
         <v>104</v>
       </c>
     </row>
@@ -2740,45 +2734,45 @@
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A78" s="29" t="s">
+      <c r="A78" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="B78" s="29"/>
-      <c r="C78" s="29"/>
-      <c r="D78" s="29"/>
-      <c r="E78" s="29"/>
-      <c r="F78" s="29"/>
-      <c r="G78" s="29"/>
-      <c r="H78" s="29"/>
+      <c r="B78" s="42"/>
+      <c r="C78" s="42"/>
+      <c r="D78" s="42"/>
+      <c r="E78" s="42"/>
+      <c r="F78" s="42"/>
+      <c r="G78" s="42"/>
+      <c r="H78" s="42"/>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A79" s="27" t="s">
+      <c r="A79" s="40" t="s">
         <v>40</v>
       </c>
       <c r="B79" s="23"/>
       <c r="C79" s="23"/>
       <c r="D79" s="23"/>
-      <c r="E79" s="27" t="s">
+      <c r="E79" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="F79" s="27" t="s">
+      <c r="F79" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="G79" s="27"/>
+      <c r="G79" s="40"/>
       <c r="H79" s="23"/>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A80" s="27"/>
+      <c r="A80" s="40"/>
       <c r="B80" s="23"/>
       <c r="C80" s="23"/>
       <c r="D80" s="23"/>
-      <c r="E80" s="27"/>
-      <c r="F80" s="28"/>
-      <c r="G80" s="28"/>
+      <c r="E80" s="40"/>
+      <c r="F80" s="41"/>
+      <c r="G80" s="41"/>
       <c r="H80" s="23"/>
     </row>
     <row r="81" spans="1:17" ht="39" x14ac:dyDescent="0.25">
-      <c r="A81" s="28"/>
+      <c r="A81" s="41"/>
       <c r="B81" s="25" t="s">
         <v>48</v>
       </c>
@@ -2788,7 +2782,7 @@
       <c r="D81" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E81" s="28"/>
+      <c r="E81" s="41"/>
       <c r="F81" s="24" t="s">
         <v>43</v>
       </c>
@@ -2798,16 +2792,16 @@
       <c r="H81" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="I81" s="35" t="s">
+      <c r="I81" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="J81" s="35" t="s">
+      <c r="J81" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="K81" s="35" t="s">
+      <c r="K81" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="L81" s="35" t="s">
+      <c r="L81" s="23" t="s">
         <v>65</v>
       </c>
       <c r="M81" t="s">
@@ -2868,8 +2862,8 @@
         <f>_xlfn.XLOOKUP(C82, $A$4:$A$21, $B$4:$B$21, "not found", 1, 1)</f>
         <v>0.60109999999999997</v>
       </c>
-      <c r="M82" s="36">
-        <f>IFERROR(FORECAST(B82,K82:L82,I82:J82), L82)</f>
+      <c r="M82" s="28">
+        <f t="shared" ref="M82:M91" si="2">IFERROR(FORECAST(B82,K82:L82,I82:J82), L82)</f>
         <v>0.60184799999999994</v>
       </c>
       <c r="N82">
@@ -2881,7 +2875,7 @@
         <v>6594.4030988061986</v>
       </c>
       <c r="P82">
-        <f>M82*N82*SQRT(2*O82/$K$5)</f>
+        <f t="shared" ref="P82:P91" si="3">M82*N82*SQRT(2*O82/$K$5)</f>
         <v>3.8302298336539642E-2</v>
       </c>
     </row>
@@ -2911,35 +2905,35 @@
         <v>22</v>
       </c>
       <c r="I83">
-        <f t="shared" ref="I83:I91" si="2">_xlfn.XLOOKUP(C83, $A$4:$A$21, $A$4:$A$21, "not found", -1, 1)</f>
+        <f t="shared" ref="I83:I91" si="4">_xlfn.XLOOKUP(C83, $A$4:$A$21, $A$4:$A$21, "not found", -1, 1)</f>
         <v>25</v>
       </c>
       <c r="J83">
-        <f t="shared" ref="J83:J91" si="3">_xlfn.XLOOKUP(C83, $A$4:$A$21, $A$4:$A$21, "not found", 1, 1)</f>
+        <f t="shared" ref="J83:J91" si="5">_xlfn.XLOOKUP(C83, $A$4:$A$21, $A$4:$A$21, "not found", 1, 1)</f>
         <v>30</v>
       </c>
       <c r="K83">
-        <f t="shared" ref="K83:K91" si="4">_xlfn.XLOOKUP(C83, $A$4:$A$21, $B$4:$B$21, "not found", -1, 1)</f>
+        <f t="shared" ref="K83:K91" si="6">_xlfn.XLOOKUP(C83, $A$4:$A$21, $B$4:$B$21, "not found", -1, 1)</f>
         <v>0.60150000000000003</v>
       </c>
       <c r="L83" s="8">
-        <f t="shared" ref="L83:L91" si="5">_xlfn.XLOOKUP(C83, $A$4:$A$21, $B$4:$B$21, "not found", 1, 1)</f>
+        <f t="shared" ref="L83:L91" si="7">_xlfn.XLOOKUP(C83, $A$4:$A$21, $B$4:$B$21, "not found", 1, 1)</f>
         <v>0.60129999999999995</v>
       </c>
-      <c r="M83" s="36">
-        <f>IFERROR(FORECAST(B83,K83:L83,I83:J83), L83)</f>
+      <c r="M83" s="28">
+        <f t="shared" si="2"/>
         <v>0.60197600000000029</v>
       </c>
       <c r="N83">
-        <f t="shared" ref="N83:N91" si="6">PI()/4*($B$76/1000)^2</f>
+        <f t="shared" ref="N83:N91" si="8">PI()/4*($B$76/1000)^2</f>
         <v>5.8534939719848437E-4</v>
       </c>
       <c r="O83">
-        <f t="shared" ref="O83:O91" si="7">C83/39.37*790*9.81</f>
+        <f t="shared" ref="O83:O91" si="9">C83/39.37*790*9.81</f>
         <v>5216.4681229362459</v>
       </c>
       <c r="P83">
-        <f>M83*N83*SQRT(2*O83/$K$5)</f>
+        <f t="shared" si="3"/>
         <v>3.4073576660497186E-2</v>
       </c>
     </row>
@@ -2969,35 +2963,35 @@
         <v>22</v>
       </c>
       <c r="I84">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="J84">
+        <f t="shared" si="5"/>
+        <v>25</v>
+      </c>
+      <c r="K84">
+        <f t="shared" si="6"/>
+        <v>0.60170000000000001</v>
+      </c>
+      <c r="L84" s="8">
+        <f t="shared" si="7"/>
+        <v>0.60150000000000003</v>
+      </c>
+      <c r="M84" s="28">
         <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="J84">
+        <v>0.60206399999999993</v>
+      </c>
+      <c r="N84">
+        <f t="shared" si="8"/>
+        <v>5.8534939719848437E-4</v>
+      </c>
+      <c r="O84">
+        <f t="shared" si="9"/>
+        <v>4350.3375666751344</v>
+      </c>
+      <c r="P84">
         <f t="shared" si="3"/>
-        <v>25</v>
-      </c>
-      <c r="K84">
-        <f t="shared" si="4"/>
-        <v>0.60170000000000001</v>
-      </c>
-      <c r="L84" s="8">
-        <f t="shared" si="5"/>
-        <v>0.60150000000000003</v>
-      </c>
-      <c r="M84" s="36">
-        <f>IFERROR(FORECAST(B84,K84:L84,I84:J84), L84)</f>
-        <v>0.60206399999999993</v>
-      </c>
-      <c r="N84">
-        <f t="shared" si="6"/>
-        <v>5.8534939719848437E-4</v>
-      </c>
-      <c r="O84">
-        <f t="shared" si="7"/>
-        <v>4350.3375666751344</v>
-      </c>
-      <c r="P84">
-        <f>M84*N84*SQRT(2*O84/$K$5)</f>
         <v>3.112106179910902E-2</v>
       </c>
     </row>
@@ -3027,35 +3021,35 @@
         <v>22</v>
       </c>
       <c r="I85">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="J85">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="K85">
+        <f t="shared" si="6"/>
+        <v>0.60199999999999998</v>
+      </c>
+      <c r="L85" s="8">
+        <f t="shared" si="7"/>
+        <v>0.60170000000000001</v>
+      </c>
+      <c r="M85" s="28">
         <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
-      <c r="J85">
+        <v>0.60235399999999995</v>
+      </c>
+      <c r="N85">
+        <f t="shared" si="8"/>
+        <v>5.8534939719848437E-4</v>
+      </c>
+      <c r="O85">
+        <f t="shared" si="9"/>
+        <v>3405.4678689357388</v>
+      </c>
+      <c r="P85">
         <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-      <c r="K85">
-        <f t="shared" si="4"/>
-        <v>0.60199999999999998</v>
-      </c>
-      <c r="L85" s="8">
-        <f t="shared" si="5"/>
-        <v>0.60170000000000001</v>
-      </c>
-      <c r="M85" s="36">
-        <f>IFERROR(FORECAST(B85,K85:L85,I85:J85), L85)</f>
-        <v>0.60235399999999995</v>
-      </c>
-      <c r="N85">
-        <f t="shared" si="6"/>
-        <v>5.8534939719848437E-4</v>
-      </c>
-      <c r="O85">
-        <f t="shared" si="7"/>
-        <v>3405.4678689357388</v>
-      </c>
-      <c r="P85">
-        <f>M85*N85*SQRT(2*O85/$K$5)</f>
         <v>2.7548024447267158E-2</v>
       </c>
     </row>
@@ -3085,35 +3079,35 @@
         <v>22</v>
       </c>
       <c r="I86">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="J86">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="K86">
+        <f t="shared" si="6"/>
+        <v>0.6028</v>
+      </c>
+      <c r="L86" s="8">
+        <f t="shared" si="7"/>
+        <v>0.60199999999999998</v>
+      </c>
+      <c r="M86" s="28">
         <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="J86">
+        <v>0.60334399999999999</v>
+      </c>
+      <c r="N86">
+        <f t="shared" si="8"/>
+        <v>5.8534939719848437E-4</v>
+      </c>
+      <c r="O86">
+        <f t="shared" si="9"/>
+        <v>2539.337312674626</v>
+      </c>
+      <c r="P86">
         <f t="shared" si="3"/>
-        <v>15</v>
-      </c>
-      <c r="K86">
-        <f t="shared" si="4"/>
-        <v>0.6028</v>
-      </c>
-      <c r="L86" s="8">
-        <f t="shared" si="5"/>
-        <v>0.60199999999999998</v>
-      </c>
-      <c r="M86" s="36">
-        <f>IFERROR(FORECAST(B86,K86:L86,I86:J86), L86)</f>
-        <v>0.60334399999999999</v>
-      </c>
-      <c r="N86">
-        <f t="shared" si="6"/>
-        <v>5.8534939719848437E-4</v>
-      </c>
-      <c r="O86">
-        <f t="shared" si="7"/>
-        <v>2539.337312674626</v>
-      </c>
-      <c r="P86">
-        <f>M86*N86*SQRT(2*O86/$K$5)</f>
         <v>2.3827334563195642E-2</v>
       </c>
     </row>
@@ -3143,35 +3137,35 @@
         <v>22</v>
       </c>
       <c r="I87">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="J87">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="K87">
+        <f t="shared" si="6"/>
+        <v>0.60289999999999999</v>
+      </c>
+      <c r="L87" s="8">
+        <f t="shared" si="7"/>
+        <v>0.60289999999999999</v>
+      </c>
+      <c r="M87" s="28">
         <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="J87">
+        <v>0.60289999999999999</v>
+      </c>
+      <c r="N87">
+        <f t="shared" si="8"/>
+        <v>5.8534939719848437E-4</v>
+      </c>
+      <c r="O87">
+        <f t="shared" si="9"/>
+        <v>1771.6306832613668</v>
+      </c>
+      <c r="P87">
         <f t="shared" si="3"/>
-        <v>9</v>
-      </c>
-      <c r="K87">
-        <f t="shared" si="4"/>
-        <v>0.60289999999999999</v>
-      </c>
-      <c r="L87" s="8">
-        <f t="shared" si="5"/>
-        <v>0.60289999999999999</v>
-      </c>
-      <c r="M87" s="36">
-        <f>IFERROR(FORECAST(B87,K87:L87,I87:J87), L87)</f>
-        <v>0.60289999999999999</v>
-      </c>
-      <c r="N87">
-        <f t="shared" si="6"/>
-        <v>5.8534939719848437E-4</v>
-      </c>
-      <c r="O87">
-        <f t="shared" si="7"/>
-        <v>1771.6306832613668</v>
-      </c>
-      <c r="P87">
-        <f>M87*N87*SQRT(2*O87/$K$5)</f>
         <v>1.9887589544148841E-2</v>
       </c>
     </row>
@@ -3201,35 +3195,35 @@
         <v>22</v>
       </c>
       <c r="I88">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="J88">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="K88">
+        <f t="shared" si="6"/>
+        <v>0.60360000000000003</v>
+      </c>
+      <c r="L88" s="8">
+        <f t="shared" si="7"/>
+        <v>0.60329999999999995</v>
+      </c>
+      <c r="M88" s="28">
         <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="J88">
+        <v>0.60441000000000034</v>
+      </c>
+      <c r="N88">
+        <f t="shared" si="8"/>
+        <v>5.8534939719848437E-4</v>
+      </c>
+      <c r="O88">
+        <f t="shared" si="9"/>
+        <v>1259.8262636525278</v>
+      </c>
+      <c r="P88">
         <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="K88">
-        <f t="shared" si="4"/>
-        <v>0.60360000000000003</v>
-      </c>
-      <c r="L88" s="8">
-        <f t="shared" si="5"/>
-        <v>0.60329999999999995</v>
-      </c>
-      <c r="M88" s="36">
-        <f>IFERROR(FORECAST(B88,K88:L88,I88:J88), L88)</f>
-        <v>0.60441000000000034</v>
-      </c>
-      <c r="N88">
-        <f t="shared" si="6"/>
-        <v>5.8534939719848437E-4</v>
-      </c>
-      <c r="O88">
-        <f t="shared" si="7"/>
-        <v>1259.8262636525278</v>
-      </c>
-      <c r="P88">
-        <f>M88*N88*SQRT(2*O88/$K$5)</f>
         <v>1.6812691250692614E-2</v>
       </c>
     </row>
@@ -3259,35 +3253,35 @@
         <v>22</v>
       </c>
       <c r="I89">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="J89">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="K89">
+        <f t="shared" si="6"/>
+        <v>0.60529999999999995</v>
+      </c>
+      <c r="L89" s="8">
+        <f t="shared" si="7"/>
+        <v>0.60450000000000004</v>
+      </c>
+      <c r="M89" s="28">
         <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="J89">
+        <v>0.60601999999999989</v>
+      </c>
+      <c r="N89">
+        <f t="shared" si="8"/>
+        <v>5.8534939719848437E-4</v>
+      </c>
+      <c r="O89">
+        <f t="shared" si="9"/>
+        <v>767.70662941325895</v>
+      </c>
+      <c r="P89">
         <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="K89">
-        <f t="shared" si="4"/>
-        <v>0.60529999999999995</v>
-      </c>
-      <c r="L89" s="8">
-        <f t="shared" si="5"/>
-        <v>0.60450000000000004</v>
-      </c>
-      <c r="M89" s="36">
-        <f>IFERROR(FORECAST(B89,K89:L89,I89:J89), L89)</f>
-        <v>0.60601999999999989</v>
-      </c>
-      <c r="N89">
-        <f t="shared" si="6"/>
-        <v>5.8534939719848437E-4</v>
-      </c>
-      <c r="O89">
-        <f t="shared" si="7"/>
-        <v>767.70662941325895</v>
-      </c>
-      <c r="P89">
-        <f>M89*N89*SQRT(2*O89/$K$5)</f>
         <v>1.3159363091418302E-2</v>
       </c>
     </row>
@@ -3317,35 +3311,35 @@
         <v>22</v>
       </c>
       <c r="I90">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="J90">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="K90">
+        <f t="shared" si="6"/>
+        <v>0.60660000000000003</v>
+      </c>
+      <c r="L90" s="8">
+        <f t="shared" si="7"/>
+        <v>0.60529999999999995</v>
+      </c>
+      <c r="M90" s="28">
         <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="J90">
+        <v>0.60777000000000014</v>
+      </c>
+      <c r="N90">
+        <f t="shared" si="8"/>
+        <v>5.8534939719848437E-4</v>
+      </c>
+      <c r="O90">
+        <f t="shared" si="9"/>
+        <v>413.38049276098553</v>
+      </c>
+      <c r="P90">
         <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="K90">
-        <f t="shared" si="4"/>
-        <v>0.60660000000000003</v>
-      </c>
-      <c r="L90" s="8">
-        <f t="shared" si="5"/>
-        <v>0.60529999999999995</v>
-      </c>
-      <c r="M90" s="36">
-        <f>IFERROR(FORECAST(B90,K90:L90,I90:J90), L90)</f>
-        <v>0.60777000000000014</v>
-      </c>
-      <c r="N90">
-        <f t="shared" si="6"/>
-        <v>5.8534939719848437E-4</v>
-      </c>
-      <c r="O90">
-        <f t="shared" si="7"/>
-        <v>413.38049276098553</v>
-      </c>
-      <c r="P90">
-        <f>M90*N90*SQRT(2*O90/$K$5)</f>
         <v>9.6842170812658085E-3</v>
       </c>
     </row>
@@ -3375,35 +3369,35 @@
         <v>22</v>
       </c>
       <c r="I91" t="str">
-        <f t="shared" si="2"/>
-        <v>not found</v>
-      </c>
-      <c r="J91">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="K91" t="str">
         <f t="shared" si="4"/>
         <v>not found</v>
       </c>
+      <c r="J91">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="K91" t="str">
+        <f t="shared" si="6"/>
+        <v>not found</v>
+      </c>
       <c r="L91" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.60950000000000004</v>
       </c>
-      <c r="M91" s="36">
-        <f>IFERROR(FORECAST(B91,K91:L91,I91:J91), L91)</f>
+      <c r="M91" s="28">
+        <f t="shared" si="2"/>
         <v>0.60950000000000004</v>
       </c>
       <c r="N91">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>5.8534939719848437E-4</v>
       </c>
       <c r="O91">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>177.16306832613671</v>
       </c>
       <c r="P91">
-        <f>M91*N91*SQRT(2*O91/$K$5)</f>
+        <f t="shared" si="3"/>
         <v>6.3578543438831724E-3</v>
       </c>
     </row>
@@ -3430,7 +3424,7 @@
       <c r="I94" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="J94" s="34" t="s">
+      <c r="J94" s="27" t="s">
         <v>100</v>
       </c>
       <c r="L94" s="8"/>
@@ -3439,11 +3433,11 @@
       <c r="B95" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C95" s="41">
+      <c r="C95" s="33">
         <f>P82</f>
         <v>3.8302298336539642E-2</v>
       </c>
-      <c r="D95" s="38">
+      <c r="D95" s="30">
         <f>G82*9.81*997*0.001</f>
         <v>1662.6969000000001</v>
       </c>
@@ -3477,7 +3471,7 @@
       <c r="B96" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="C96" s="41">
+      <c r="C96" s="33">
         <f>P82</f>
         <v>3.8302298336539642E-2</v>
       </c>
@@ -3505,7 +3499,7 @@
         <f>C96*SQRT(1-G96^4)/H96*SQRT($K$5/(2*D96))</f>
         <v>0.97438003710767163</v>
       </c>
-      <c r="J96" s="41">
+      <c r="J96" s="33">
         <f>0.9965-6.53*SQRT(G96/L99)</f>
         <v>0.97731471248443691</v>
       </c>
@@ -3514,7 +3508,7 @@
       <c r="K97" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="L97" s="39">
+      <c r="L97" s="31">
         <f>0.0000018347*10</f>
         <v>1.8346999999999999E-5</v>
       </c>
@@ -3532,24 +3526,24 @@
       <c r="K99" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="L99" s="38">
+      <c r="L99" s="30">
         <f>L98*$K$5*D76/1000/L97</f>
         <v>39754.919311494705</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="J46:J48"/>
-    <mergeCell ref="N46:N48"/>
-    <mergeCell ref="O46:P47"/>
-    <mergeCell ref="F79:G80"/>
-    <mergeCell ref="A78:H78"/>
     <mergeCell ref="A26:A30"/>
     <mergeCell ref="A32:A36"/>
     <mergeCell ref="A24:D24"/>
     <mergeCell ref="A41:A45"/>
     <mergeCell ref="A47:A51"/>
     <mergeCell ref="A39:D39"/>
+    <mergeCell ref="J46:J48"/>
+    <mergeCell ref="N46:N48"/>
+    <mergeCell ref="O46:P47"/>
+    <mergeCell ref="F79:G80"/>
+    <mergeCell ref="A78:H78"/>
     <mergeCell ref="A54:B54"/>
     <mergeCell ref="A68:E68"/>
     <mergeCell ref="A74:C74"/>

</xml_diff>